<commit_message>
Added Malaysian PINT doc types; TICC-312
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.8.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6534B923-F4D2-4656-9FBF-69CAD06E6ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD45B871-85A7-4D72-B83D-6F2AC92349EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="670">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2071,6 +2071,33 @@
   <si>
     <t>TICC-155
 TICC-304</t>
+  </si>
+  <si>
+    <t>MY PINT Invoice v1.0</t>
+  </si>
+  <si>
+    <t>MY PINT Credit Note v1.0</t>
+  </si>
+  <si>
+    <t>MY PINT Self-Billing Invoice v1.0</t>
+  </si>
+  <si>
+    <t>MY PINT Self-Billing Credit Note v1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:billing-1@my-1::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:billing-1@my-1::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:selfbilling-1@my-1::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:selfbilling-1@my-1::2.1</t>
+  </si>
+  <si>
+    <t>TICC-312</t>
   </si>
 </sst>
 </file>
@@ -2730,11 +2757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L245"/>
+  <dimension ref="A1:L249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F103" sqref="F103"/>
+      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A250" sqref="A250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9737,7 +9764,7 @@
       <c r="B220" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="1" t="s">
         <v>602</v>
       </c>
       <c r="D220" s="28" t="s">
@@ -10533,6 +10560,134 @@
       </c>
       <c r="L245" s="5" t="s">
         <v>616</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>661</v>
+      </c>
+      <c r="B246" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D246" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E246" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H246" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="I246" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J246" s="24">
+        <v>3</v>
+      </c>
+      <c r="K246" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L246" s="5" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>662</v>
+      </c>
+      <c r="B247" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D247" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E247" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H247" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="I247" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J247" s="24">
+        <v>3</v>
+      </c>
+      <c r="K247" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L247" s="5" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>663</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="D248" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E248" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H248" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="I248" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J248" s="24">
+        <v>3</v>
+      </c>
+      <c r="K248" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L248" s="5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>664</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D249" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E249" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H249" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="I249" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J249" s="24">
+        <v>3</v>
+      </c>
+      <c r="K249" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L249" s="5" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>